<commit_message>
Generalize visualizations to experiment_visualizer
</commit_message>
<xml_diff>
--- a/experiment_results/manual_vs_high-level.xlsx
+++ b/experiment_results/manual_vs_high-level.xlsx
@@ -493,7 +493,7 @@
         <v>141</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>0</v>
@@ -513,7 +513,7 @@
         <v>137</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>0</v>
@@ -533,7 +533,7 @@
         <v>170</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>0</v>
@@ -553,7 +553,7 @@
         <v>170</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>0</v>
@@ -577,7 +577,7 @@
         <v>290</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>5</v>
@@ -597,7 +597,7 @@
         <v>193</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>0</v>
@@ -617,7 +617,7 @@
         <v>421</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>17</v>
@@ -637,7 +637,7 @@
         <v>236</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>0</v>
@@ -661,7 +661,7 @@
         <v>753</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="F10" s="3" t="n">
         <v>17</v>
@@ -681,7 +681,7 @@
         <v>122</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="3" t="n">
         <v>0</v>
@@ -701,7 +701,7 @@
         <v>805</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F12" s="3" t="n">
         <v>18</v>
@@ -721,7 +721,7 @@
         <v>183</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F13" s="3" t="n">
         <v>0</v>
@@ -745,7 +745,7 @@
         <v>276</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="F14" s="3" t="n">
         <v>6</v>
@@ -765,7 +765,7 @@
         <v>73</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="3" t="n">
         <v>0</v>
@@ -785,7 +785,7 @@
         <v>339</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F16" s="3" t="n">
         <v>8</v>
@@ -805,7 +805,7 @@
         <v>119</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F17" s="3" t="n">
         <v>0</v>
@@ -829,7 +829,7 @@
         <v>541</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F18" s="3" t="n">
         <v>7</v>
@@ -849,7 +849,7 @@
         <v>295</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F19" s="3" t="n">
         <v>0</v>
@@ -869,7 +869,7 @@
         <v>897</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="F20" s="3" t="n">
         <v>18</v>
@@ -889,7 +889,7 @@
         <v>201</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="3" t="n">
         <v>0</v>
@@ -913,7 +913,7 @@
         <v>643</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F22" s="3" t="n">
         <v>13</v>
@@ -933,7 +933,7 @@
         <v>338</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="F23" s="3" t="n">
         <v>0</v>
@@ -953,7 +953,7 @@
         <v>1422</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F24" s="3" t="n">
         <v>23</v>
@@ -973,7 +973,7 @@
         <v>439</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="F25" s="3" t="n">
         <v>0</v>
@@ -997,7 +997,7 @@
         <v>798</v>
       </c>
       <c r="E26" s="3" t="n">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="F26" s="3" t="n">
         <v>18</v>
@@ -1017,7 +1017,7 @@
         <v>164</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="3" t="n">
         <v>0</v>
@@ -1037,7 +1037,7 @@
         <v>824</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F28" s="3" t="n">
         <v>19</v>
@@ -1057,7 +1057,7 @@
         <v>192</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F29" s="3" t="n">
         <v>0</v>
@@ -1081,7 +1081,7 @@
         <v>421</v>
       </c>
       <c r="E30" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F30" s="3" t="n">
         <v>5</v>
@@ -1101,7 +1101,7 @@
         <v>171</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F31" s="3" t="n">
         <v>0</v>
@@ -1121,7 +1121,7 @@
         <v>320</v>
       </c>
       <c r="E32" s="3" t="n">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="F32" s="3" t="n">
         <v>6</v>
@@ -1141,7 +1141,7 @@
         <v>176</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F33" s="3" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Update count complexity in runner. Add diagram file generation in visualizer
Also add the diagrams for Test 1
</commit_message>
<xml_diff>
--- a/experiment_results/manual_vs_high-level.xlsx
+++ b/experiment_results/manual_vs_high-level.xlsx
@@ -493,7 +493,7 @@
         <v>141</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>0</v>
@@ -513,7 +513,7 @@
         <v>137</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>0</v>
@@ -533,7 +533,7 @@
         <v>170</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>0</v>
@@ -553,7 +553,7 @@
         <v>170</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>0</v>
@@ -577,7 +577,7 @@
         <v>290</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>2</v>
+        <v>5.5</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>5</v>
@@ -597,7 +597,7 @@
         <v>193</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>0</v>
@@ -617,7 +617,7 @@
         <v>421</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>17</v>
@@ -637,7 +637,7 @@
         <v>236</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>0</v>
@@ -661,7 +661,7 @@
         <v>753</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>6.5</v>
+        <v>19.5</v>
       </c>
       <c r="F10" s="3" t="n">
         <v>17</v>
@@ -681,7 +681,7 @@
         <v>122</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F11" s="3" t="n">
         <v>0</v>
@@ -701,7 +701,7 @@
         <v>805</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>7</v>
+        <v>19.5</v>
       </c>
       <c r="F12" s="3" t="n">
         <v>18</v>
@@ -721,7 +721,7 @@
         <v>183</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="F13" s="3" t="n">
         <v>0</v>
@@ -745,7 +745,7 @@
         <v>276</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="F14" s="3" t="n">
         <v>6</v>
@@ -785,7 +785,7 @@
         <v>339</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>4</v>
+        <v>6.5</v>
       </c>
       <c r="F16" s="3" t="n">
         <v>8</v>
@@ -829,7 +829,7 @@
         <v>541</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>4</v>
+        <v>12.5</v>
       </c>
       <c r="F18" s="3" t="n">
         <v>7</v>
@@ -849,7 +849,7 @@
         <v>295</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="F19" s="3" t="n">
         <v>0</v>
@@ -869,7 +869,7 @@
         <v>897</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>7.5</v>
+        <v>22.5</v>
       </c>
       <c r="F20" s="3" t="n">
         <v>18</v>
@@ -889,7 +889,7 @@
         <v>201</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="F21" s="3" t="n">
         <v>0</v>
@@ -913,7 +913,7 @@
         <v>643</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F22" s="3" t="n">
         <v>13</v>
@@ -933,7 +933,7 @@
         <v>338</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="F23" s="3" t="n">
         <v>0</v>
@@ -953,7 +953,7 @@
         <v>1422</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>9</v>
+        <v>41.5</v>
       </c>
       <c r="F24" s="3" t="n">
         <v>23</v>
@@ -973,7 +973,7 @@
         <v>439</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>2.5</v>
+        <v>7.5</v>
       </c>
       <c r="F25" s="3" t="n">
         <v>0</v>
@@ -997,7 +997,7 @@
         <v>798</v>
       </c>
       <c r="E26" s="3" t="n">
-        <v>7.5</v>
+        <v>17.5</v>
       </c>
       <c r="F26" s="3" t="n">
         <v>18</v>
@@ -1017,7 +1017,7 @@
         <v>164</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="3" t="n">
         <v>0</v>
@@ -1037,7 +1037,7 @@
         <v>824</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>8</v>
+        <v>18.5</v>
       </c>
       <c r="F28" s="3" t="n">
         <v>19</v>
@@ -1057,7 +1057,7 @@
         <v>192</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="F29" s="3" t="n">
         <v>0</v>
@@ -1081,7 +1081,7 @@
         <v>421</v>
       </c>
       <c r="E30" s="3" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F30" s="3" t="n">
         <v>5</v>
@@ -1101,7 +1101,7 @@
         <v>171</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="F31" s="3" t="n">
         <v>0</v>
@@ -1121,7 +1121,7 @@
         <v>320</v>
       </c>
       <c r="E32" s="3" t="n">
-        <v>3.5</v>
+        <v>8.5</v>
       </c>
       <c r="F32" s="3" t="n">
         <v>6</v>
@@ -1141,7 +1141,7 @@
         <v>176</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F33" s="3" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Update count_complexity. Update experiments according to the DISCLAIMER note
</commit_message>
<xml_diff>
--- a/experiment_results/manual_vs_high-level.xlsx
+++ b/experiment_results/manual_vs_high-level.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Experiment Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Experiment Results" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -483,17 +483,17 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>manual_test_simple_2</t>
+          <t>manual_test_join_1</t>
         </is>
       </c>
       <c r="C2" s="3" t="n">
         <v>3</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>0</v>
@@ -503,7 +503,7 @@
       <c r="A3" s="3" t="n"/>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>high_level_test_simple_2</t>
+          <t>high_level_test_join_1</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
@@ -513,7 +513,7 @@
         <v>137</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>0</v>
@@ -523,17 +523,17 @@
       <c r="A4" s="3" t="n"/>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>manual_test_join_1</t>
+          <t>manual_test_join_2</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
         <v>3</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>3.5</v>
+        <v>1.5</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>0</v>
@@ -543,7 +543,7 @@
       <c r="A5" s="3" t="n"/>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>high_level_test_join_1</t>
+          <t>high_level_test_join_2</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
@@ -553,7 +553,7 @@
         <v>170</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>3.5</v>
+        <v>1.5</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>0</v>
@@ -577,7 +577,7 @@
         <v>290</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>5.5</v>
+        <v>2</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>5</v>
@@ -597,7 +597,7 @@
         <v>193</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>3.5</v>
+        <v>1.5</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>0</v>
@@ -617,7 +617,7 @@
         <v>421</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>17</v>
@@ -637,7 +637,7 @@
         <v>236</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>0</v>
@@ -661,7 +661,7 @@
         <v>753</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>19.5</v>
+        <v>6.5</v>
       </c>
       <c r="F10" s="3" t="n">
         <v>17</v>
@@ -681,7 +681,7 @@
         <v>122</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F11" s="3" t="n">
         <v>0</v>
@@ -701,7 +701,7 @@
         <v>805</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>19.5</v>
+        <v>7</v>
       </c>
       <c r="F12" s="3" t="n">
         <v>18</v>
@@ -721,7 +721,7 @@
         <v>183</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="F13" s="3" t="n">
         <v>0</v>
@@ -745,7 +745,7 @@
         <v>276</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>5.5</v>
+        <v>3.5</v>
       </c>
       <c r="F14" s="3" t="n">
         <v>6</v>
@@ -785,7 +785,7 @@
         <v>339</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="F16" s="3" t="n">
         <v>8</v>
@@ -829,7 +829,7 @@
         <v>541</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>12.5</v>
+        <v>4</v>
       </c>
       <c r="F18" s="3" t="n">
         <v>7</v>
@@ -849,7 +849,7 @@
         <v>295</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="F19" s="3" t="n">
         <v>0</v>
@@ -869,7 +869,7 @@
         <v>897</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>22.5</v>
+        <v>7.5</v>
       </c>
       <c r="F20" s="3" t="n">
         <v>18</v>
@@ -889,7 +889,7 @@
         <v>201</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="F21" s="3" t="n">
         <v>0</v>
@@ -913,7 +913,7 @@
         <v>643</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F22" s="3" t="n">
         <v>13</v>
@@ -933,7 +933,7 @@
         <v>338</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>5.5</v>
+        <v>2.5</v>
       </c>
       <c r="F23" s="3" t="n">
         <v>0</v>
@@ -953,7 +953,7 @@
         <v>1422</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>41.5</v>
+        <v>9</v>
       </c>
       <c r="F24" s="3" t="n">
         <v>23</v>
@@ -973,7 +973,7 @@
         <v>439</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>7.5</v>
+        <v>2.5</v>
       </c>
       <c r="F25" s="3" t="n">
         <v>0</v>
@@ -997,7 +997,7 @@
         <v>798</v>
       </c>
       <c r="E26" s="3" t="n">
-        <v>17.5</v>
+        <v>7.5</v>
       </c>
       <c r="F26" s="3" t="n">
         <v>18</v>
@@ -1017,7 +1017,7 @@
         <v>164</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" s="3" t="n">
         <v>0</v>
@@ -1037,7 +1037,7 @@
         <v>824</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>18.5</v>
+        <v>8</v>
       </c>
       <c r="F28" s="3" t="n">
         <v>19</v>
@@ -1057,7 +1057,7 @@
         <v>192</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="F29" s="3" t="n">
         <v>0</v>
@@ -1081,7 +1081,7 @@
         <v>421</v>
       </c>
       <c r="E30" s="3" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F30" s="3" t="n">
         <v>5</v>
@@ -1101,7 +1101,7 @@
         <v>171</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>3.5</v>
+        <v>1.5</v>
       </c>
       <c r="F31" s="3" t="n">
         <v>0</v>
@@ -1121,7 +1121,7 @@
         <v>320</v>
       </c>
       <c r="E32" s="3" t="n">
-        <v>8.5</v>
+        <v>3.5</v>
       </c>
       <c r="F32" s="3" t="n">
         <v>6</v>
@@ -1141,7 +1141,7 @@
         <v>176</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F33" s="3" t="n">
         <v>0</v>

</xml_diff>